<commit_message>
Reads multiple excel sheets
Reads multiple excel sheets and stores to ATS
</commit_message>
<xml_diff>
--- a/importDataPoc/src/main/resources/testExcel.xlsx
+++ b/importDataPoc/src/main/resources/testExcel.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11009"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aruddha.roy/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aruddha.roy/Desktop/Application_Code_Poc/importDataPoc/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F5402D63-8CA0-524A-81CF-704704EB2F36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{525D54AC-A290-7F47-8FF3-9DA67AF0D606}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3260" yWindow="2160" windowWidth="28040" windowHeight="17440" xr2:uid="{B0CB5A7B-A4D7-7A42-BC64-850F2F2076AB}"/>
+    <workbookView xWindow="6520" yWindow="2640" windowWidth="28040" windowHeight="17440" xr2:uid="{B0CB5A7B-A4D7-7A42-BC64-850F2F2076AB}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -463,7 +463,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>